<commit_message>
Add function for matched cards
</commit_message>
<xml_diff>
--- a/demon list and cards.xlsx
+++ b/demon list and cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\projects\game_project\cardSlayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA77E27C-94F3-4D41-9CEC-38C44284E203}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340BB8BC-75C4-444F-B1D5-6623DF9640B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="18810" windowHeight="9810" xr2:uid="{B72EA5E1-FF28-425C-BF6F-E34603362299}"/>
+    <workbookView xWindow="15" yWindow="0" windowWidth="19185" windowHeight="10200" xr2:uid="{B72EA5E1-FF28-425C-BF6F-E34603362299}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Update list of damages in Excel file
</commit_message>
<xml_diff>
--- a/demon list and cards.xlsx
+++ b/demon list and cards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mitch\projects\game_project\cardSlayer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{340BB8BC-75C4-444F-B1D5-6623DF9640B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F323037B-D1E7-4B2D-8D6B-B60F4FF463EE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="19185" windowHeight="10200" xr2:uid="{B72EA5E1-FF28-425C-BF6F-E34603362299}"/>
+    <workbookView xWindow="1200" yWindow="1485" windowWidth="13395" windowHeight="10200" xr2:uid="{B72EA5E1-FF28-425C-BF6F-E34603362299}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>hit points</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Cyberdemon</t>
+  </si>
+  <si>
+    <t>lessHealth</t>
+  </si>
+  <si>
+    <t>minNumOfMoves</t>
+  </si>
+  <si>
+    <t>giveChance</t>
+  </si>
+  <si>
+    <t>with rounding</t>
   </si>
 </sst>
 </file>
@@ -421,20 +433,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{129488B9-B63B-4652-80BE-BBC48874CA5E}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -447,8 +461,20 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -462,8 +488,20 @@
       <c r="D2">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <f>D2/2</f>
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <f>(100/D2)</f>
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <f>ROUNDUP(G2,0)</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -477,8 +515,20 @@
       <c r="D3">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <f t="shared" ref="E3:E13" si="1">D3/2</f>
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G13" si="2">(100/D3)</f>
+        <v>16.666666666666668</v>
+      </c>
+      <c r="H3">
+        <f>ROUNDUP(G3,0)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -492,8 +542,20 @@
       <c r="D4">
         <v>8</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>12.5</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H13" si="3">ROUNDUP(G4,0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -507,8 +569,20 @@
       <c r="D5">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>8.3333333333333339</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -522,8 +596,20 @@
       <c r="D6">
         <v>16</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>6.25</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -537,8 +623,20 @@
       <c r="D7">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -552,8 +650,20 @@
       <c r="D8">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>12.5</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -567,8 +677,20 @@
       <c r="D9">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>3.3333333333333335</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -582,8 +704,20 @@
       <c r="D10">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>2.7777777777777777</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -597,8 +731,20 @@
       <c r="D11">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>2.5</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -612,8 +758,20 @@
       <c r="D12">
         <v>49</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>24.5</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>2.0408163265306123</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -626,6 +784,18 @@
       </c>
       <c r="D13">
         <v>64</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>1.5625</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>